<commit_message>
Planificación 001 añadida - NBQ_050100
</commit_message>
<xml_diff>
--- a/ControlCambios/05_Planificacion/Plan_001.xlsx
+++ b/ControlCambios/05_Planificacion/Plan_001.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nubeusc-my.sharepoint.com/personal/roi_martinez_enriquez_rai_usc_es/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Niko\Documents\Uni\EnSo\EnSo_ControlCambios_gr1.2\ControlCambios\05_Planificacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FC2287AE-51C0-4228-85B9-83AB943B046D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D29C2312-1EC8-4351-991C-380F62AE2D0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{A0B7CE81-5765-4616-ABB9-45231285591F}"/>
+    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{A0B7CE81-5765-4616-ABB9-45231285591F}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
     <t xml:space="preserve">ID: </t>
   </si>
@@ -59,89 +59,92 @@
     <t>Nombre:</t>
   </si>
   <si>
-    <t>[Introduzca el nombre completo]</t>
-  </si>
-  <si>
     <t>Correo:</t>
   </si>
   <si>
-    <t>[Introduzca el correo electrónico]</t>
-  </si>
-  <si>
     <t>ID Empleado:</t>
   </si>
   <si>
-    <t>[Número de empleado asignado al gerente]</t>
-  </si>
-  <si>
     <t>Planificación</t>
   </si>
   <si>
     <t>Tiempo estimado:</t>
   </si>
   <si>
-    <t>[Proporcione una estimación del tiempo estimado de la ejecución de la  planificación]</t>
-  </si>
-  <si>
     <t>Recursos requeridos:</t>
   </si>
   <si>
-    <t>[Indique los recursos necesarios para ejecutar la planificación]</t>
-  </si>
-  <si>
     <t>Definición de tareas y actividades:</t>
   </si>
   <si>
-    <t>[Especifique las tareas y actividades que constituyen la planificación]</t>
-  </si>
-  <si>
     <t>Medidas de mitigación:</t>
   </si>
   <si>
-    <t>[De haber, especifique las medidas de mitigación para los posibles riesgos identificados]</t>
-  </si>
-  <si>
     <t>Poker Scrum</t>
   </si>
   <si>
     <t>Tiempo Mínimo</t>
   </si>
   <si>
-    <t>[Indique el nombre del dueño de la estimación]</t>
-  </si>
-  <si>
-    <t>[Valor y justificación de la decisión de tiempo mínimo]</t>
-  </si>
-  <si>
     <t>Tiempo Máximo</t>
   </si>
   <si>
-    <t>[Valor y justificación de la decisión de tiempo máximo]</t>
-  </si>
-  <si>
     <t>Tiempo más probable</t>
   </si>
   <si>
-    <t>[Indique el valor y el número de veces que se repitió]</t>
-  </si>
-  <si>
     <t>Tiempo Medio</t>
   </si>
   <si>
-    <t>[Resultado de aplicar la fórmula (Tmin + 4Tprob + Tmax)/6]</t>
-  </si>
-  <si>
     <t>PLANIFICACIÓN</t>
   </si>
   <si>
     <t>1/1</t>
+  </si>
+  <si>
+    <t>Nicolás Barcia Quintela</t>
+  </si>
+  <si>
+    <t>nicolas.barcia@rai.usc.es</t>
+  </si>
+  <si>
+    <t>NBQ_050100</t>
+  </si>
+  <si>
+    <t>1 semana</t>
+  </si>
+  <si>
+    <t>Gerente del proyecto, equipo de desarrollo</t>
+  </si>
+  <si>
+    <t>1 semana: Repetido 2 veces</t>
+  </si>
+  <si>
+    <t>Jesús Campos</t>
+  </si>
+  <si>
+    <t>3 días: Mediante el uso de librerías puede ser fácil de implementar esta medida</t>
+  </si>
+  <si>
+    <t>Roi Martínez</t>
+  </si>
+  <si>
+    <t>13 días: Puede ser complicado asegurar la protección y seguridad de los datos, así como la implementación en distintos sistemas operativos.</t>
+  </si>
+  <si>
+    <t>Selección de librería de generación de PDFs, diseño de plantilla, desarrollo backend, desarrollo frontend</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Implementar medidas para el manejo de grandes volúmenes de datos, colaborar con expertos en múltiples sistemas operativos. </t>
+  </si>
+  <si>
+    <t>7.33 días</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -210,6 +213,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -634,10 +645,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -651,24 +663,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
@@ -678,12 +672,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
@@ -692,81 +680,118 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="5"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="7" fillId="2" borderId="32" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="7" fillId="2" borderId="32" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -783,9 +808,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - Tema de 2022">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -823,7 +848,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -929,7 +954,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1071,7 +1096,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1081,14 +1106,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50348CFE-78AC-4183-AE37-6C1BCA731247}">
   <dimension ref="C2:P46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="F37" sqref="F37:I37"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F38" sqref="F38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="2" spans="3:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="3:13" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="3" spans="3:13" x14ac:dyDescent="0.3">
       <c r="C3" s="1" t="s">
         <v>0</v>
       </c>
@@ -1102,409 +1127,429 @@
         <v>2</v>
       </c>
       <c r="I3" s="5">
-        <v>45323</v>
+        <v>45349</v>
       </c>
       <c r="J3" s="6"/>
     </row>
-    <row r="4" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C4" s="7" t="s">
+    <row r="4" spans="3:13" x14ac:dyDescent="0.3">
+      <c r="C4" s="50" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="8"/>
-      <c r="E4" s="8"/>
-      <c r="F4" s="8"/>
-      <c r="G4" s="9" t="s">
+      <c r="D4" s="51"/>
+      <c r="E4" s="51"/>
+      <c r="F4" s="51"/>
+      <c r="G4" s="52" t="s">
         <v>4</v>
       </c>
-      <c r="H4" s="9"/>
-      <c r="I4" s="9"/>
-      <c r="J4" s="10"/>
-    </row>
-    <row r="5" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C5" s="11" t="s">
+      <c r="H4" s="52"/>
+      <c r="I4" s="52"/>
+      <c r="J4" s="53"/>
+    </row>
+    <row r="5" spans="3:13" x14ac:dyDescent="0.3">
+      <c r="C5" s="43" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="12"/>
-      <c r="J5" s="13"/>
-    </row>
-    <row r="6" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C6" s="14"/>
-      <c r="J6" s="13"/>
-    </row>
-    <row r="7" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C7" s="15" t="s">
+      <c r="D5" s="44"/>
+      <c r="J5" s="7"/>
+    </row>
+    <row r="6" spans="3:13" x14ac:dyDescent="0.3">
+      <c r="C6" s="8"/>
+      <c r="J6" s="7"/>
+    </row>
+    <row r="7" spans="3:13" x14ac:dyDescent="0.3">
+      <c r="C7" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="16"/>
-      <c r="E7" s="16"/>
-      <c r="F7" s="17" t="s">
+      <c r="D7" s="34"/>
+      <c r="E7" s="34"/>
+      <c r="F7" s="54" t="s">
+        <v>21</v>
+      </c>
+      <c r="G7" s="54"/>
+      <c r="H7" s="54"/>
+      <c r="I7" s="54"/>
+      <c r="J7" s="7"/>
+    </row>
+    <row r="8" spans="3:13" x14ac:dyDescent="0.3">
+      <c r="C8" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="G7" s="17"/>
-      <c r="H7" s="17"/>
-      <c r="I7" s="17"/>
-      <c r="J7" s="13"/>
-    </row>
-    <row r="8" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C8" s="15" t="s">
+      <c r="D8" s="34"/>
+      <c r="E8" s="34"/>
+      <c r="F8" s="55" t="s">
+        <v>22</v>
+      </c>
+      <c r="G8" s="54"/>
+      <c r="H8" s="54"/>
+      <c r="I8" s="54"/>
+      <c r="J8" s="7"/>
+    </row>
+    <row r="9" spans="3:13" x14ac:dyDescent="0.3">
+      <c r="C9" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="16"/>
-      <c r="E8" s="16"/>
-      <c r="F8" s="17" t="s">
+      <c r="D9" s="34"/>
+      <c r="E9" s="34"/>
+      <c r="F9" s="41" t="s">
+        <v>23</v>
+      </c>
+      <c r="G9" s="42"/>
+      <c r="H9" s="42"/>
+      <c r="I9" s="42"/>
+      <c r="J9" s="7"/>
+    </row>
+    <row r="10" spans="3:13" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="C10" s="12"/>
+      <c r="D10" s="13"/>
+      <c r="E10" s="13"/>
+      <c r="F10" s="13"/>
+      <c r="G10" s="13"/>
+      <c r="H10" s="13"/>
+      <c r="I10" s="13"/>
+      <c r="J10" s="14"/>
+      <c r="M10" s="15"/>
+    </row>
+    <row r="11" spans="3:13" x14ac:dyDescent="0.3">
+      <c r="C11" s="43" t="s">
         <v>9</v>
       </c>
-      <c r="G8" s="17"/>
-      <c r="H8" s="17"/>
-      <c r="I8" s="17"/>
-      <c r="J8" s="13"/>
-    </row>
-    <row r="9" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C9" s="15" t="s">
+      <c r="D11" s="44"/>
+      <c r="J11" s="7"/>
+    </row>
+    <row r="12" spans="3:13" x14ac:dyDescent="0.3">
+      <c r="C12" s="8"/>
+      <c r="J12" s="7"/>
+    </row>
+    <row r="13" spans="3:13" x14ac:dyDescent="0.3">
+      <c r="C13" s="33" t="s">
         <v>10</v>
       </c>
-      <c r="D9" s="16"/>
-      <c r="E9" s="16"/>
-      <c r="F9" s="18" t="s">
+      <c r="D13" s="34"/>
+      <c r="E13" s="45"/>
+      <c r="F13" s="59" t="s">
+        <v>24</v>
+      </c>
+      <c r="G13" s="60"/>
+      <c r="H13" s="60"/>
+      <c r="I13" s="60"/>
+      <c r="J13" s="16"/>
+    </row>
+    <row r="14" spans="3:13" x14ac:dyDescent="0.3">
+      <c r="C14" s="9"/>
+      <c r="D14" s="10"/>
+      <c r="E14" s="10"/>
+      <c r="F14" s="60"/>
+      <c r="G14" s="60"/>
+      <c r="H14" s="60"/>
+      <c r="I14" s="60"/>
+      <c r="J14" s="16"/>
+    </row>
+    <row r="15" spans="3:13" x14ac:dyDescent="0.3">
+      <c r="C15" s="9"/>
+      <c r="D15" s="10"/>
+      <c r="E15" s="10"/>
+      <c r="J15" s="7"/>
+    </row>
+    <row r="16" spans="3:13" x14ac:dyDescent="0.3">
+      <c r="C16" s="33" t="s">
         <v>11</v>
       </c>
-      <c r="G9" s="19"/>
-      <c r="H9" s="19"/>
-      <c r="I9" s="19"/>
-      <c r="J9" s="13"/>
-    </row>
-    <row r="10" spans="3:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C10" s="20"/>
-      <c r="D10" s="21"/>
-      <c r="E10" s="21"/>
-      <c r="F10" s="21"/>
-      <c r="G10" s="21"/>
-      <c r="H10" s="21"/>
-      <c r="I10" s="21"/>
-      <c r="J10" s="22"/>
-      <c r="M10" s="23"/>
-    </row>
-    <row r="11" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C11" s="11" t="s">
+      <c r="D16" s="34"/>
+      <c r="E16" s="46"/>
+      <c r="F16" s="47" t="s">
+        <v>25</v>
+      </c>
+      <c r="G16" s="48"/>
+      <c r="H16" s="48"/>
+      <c r="I16" s="49"/>
+      <c r="J16" s="7"/>
+    </row>
+    <row r="17" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C17" s="9"/>
+      <c r="D17" s="10"/>
+      <c r="E17" s="10"/>
+      <c r="F17" s="11"/>
+      <c r="G17" s="11"/>
+      <c r="H17" s="11"/>
+      <c r="I17" s="11"/>
+      <c r="J17" s="7"/>
+    </row>
+    <row r="18" spans="3:12" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C18" s="9"/>
+      <c r="D18" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="D11" s="12"/>
-      <c r="J11" s="13"/>
-    </row>
-    <row r="12" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C12" s="14"/>
-      <c r="J12" s="13"/>
-    </row>
-    <row r="13" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C13" s="15" t="s">
+      <c r="E18" s="10"/>
+      <c r="F18" s="56" t="s">
+        <v>31</v>
+      </c>
+      <c r="G18" s="57"/>
+      <c r="H18" s="57"/>
+      <c r="I18" s="58"/>
+      <c r="J18" s="7"/>
+    </row>
+    <row r="19" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C19" s="9"/>
+      <c r="D19" s="10"/>
+      <c r="E19" s="10"/>
+      <c r="F19" s="11"/>
+      <c r="G19" s="11"/>
+      <c r="H19" s="11"/>
+      <c r="I19" s="11"/>
+      <c r="J19" s="17"/>
+    </row>
+    <row r="20" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C20" s="9"/>
+      <c r="D20" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="D13" s="16"/>
-      <c r="E13" s="24"/>
-      <c r="F13" s="25" t="s">
+      <c r="E20" s="10"/>
+      <c r="F20" s="38" t="s">
+        <v>32</v>
+      </c>
+      <c r="G20" s="38"/>
+      <c r="H20" s="38"/>
+      <c r="I20" s="38"/>
+      <c r="J20" s="18"/>
+      <c r="L20" s="19"/>
+    </row>
+    <row r="21" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C21" s="9"/>
+      <c r="D21" s="10"/>
+      <c r="E21" s="10"/>
+      <c r="F21" s="38"/>
+      <c r="G21" s="38"/>
+      <c r="H21" s="38"/>
+      <c r="I21" s="38"/>
+      <c r="J21" s="20"/>
+      <c r="L21" s="21"/>
+    </row>
+    <row r="22" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C22" s="8"/>
+      <c r="J22" s="7"/>
+      <c r="L22" s="21"/>
+    </row>
+    <row r="23" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C23" s="39" t="s">
         <v>14</v>
       </c>
-      <c r="G13" s="26"/>
-      <c r="H13" s="26"/>
-      <c r="I13" s="26"/>
-      <c r="J13" s="27"/>
-    </row>
-    <row r="14" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C14" s="28"/>
-      <c r="D14" s="29"/>
-      <c r="E14" s="29"/>
-      <c r="F14" s="26"/>
-      <c r="G14" s="26"/>
-      <c r="H14" s="26"/>
-      <c r="I14" s="26"/>
-      <c r="J14" s="27"/>
-    </row>
-    <row r="15" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C15" s="28"/>
-      <c r="D15" s="29"/>
-      <c r="E15" s="29"/>
-      <c r="J15" s="13"/>
-    </row>
-    <row r="16" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C16" s="15" t="s">
+      <c r="D23" s="40"/>
+      <c r="E23" s="22"/>
+      <c r="F23" s="22"/>
+      <c r="G23" s="22"/>
+      <c r="H23" s="22"/>
+      <c r="I23" s="22"/>
+      <c r="J23" s="23"/>
+      <c r="L23" s="21"/>
+    </row>
+    <row r="24" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C24" s="8"/>
+      <c r="J24" s="7"/>
+      <c r="L24" s="21"/>
+    </row>
+    <row r="25" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C25" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="D16" s="16"/>
-      <c r="E16" s="30"/>
-      <c r="F16" s="31" t="s">
-        <v>16</v>
-      </c>
-      <c r="G16" s="32"/>
-      <c r="H16" s="32"/>
-      <c r="I16" s="33"/>
-      <c r="J16" s="13"/>
-    </row>
-    <row r="17" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C17" s="28"/>
-      <c r="D17" s="29"/>
-      <c r="E17" s="29"/>
-      <c r="F17" s="34"/>
-      <c r="G17" s="34"/>
-      <c r="H17" s="34"/>
-      <c r="I17" s="34"/>
-      <c r="J17" s="13"/>
-    </row>
-    <row r="18" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C18" s="28"/>
-      <c r="D18" s="29" t="s">
-        <v>17</v>
-      </c>
-      <c r="E18" s="29"/>
-      <c r="F18" s="35" t="s">
-        <v>18</v>
-      </c>
-      <c r="G18" s="36"/>
-      <c r="H18" s="36"/>
-      <c r="I18" s="37"/>
-      <c r="J18" s="13"/>
-    </row>
-    <row r="19" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C19" s="28"/>
-      <c r="D19" s="29"/>
-      <c r="E19" s="29"/>
-      <c r="F19" s="34"/>
-      <c r="G19" s="34"/>
-      <c r="H19" s="34"/>
-      <c r="I19" s="34"/>
-      <c r="J19" s="38"/>
-    </row>
-    <row r="20" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C20" s="28"/>
-      <c r="D20" s="29" t="s">
-        <v>19</v>
-      </c>
-      <c r="E20" s="29"/>
-      <c r="F20" s="39" t="s">
-        <v>20</v>
-      </c>
-      <c r="G20" s="39"/>
-      <c r="H20" s="39"/>
-      <c r="I20" s="39"/>
-      <c r="J20" s="40"/>
-      <c r="L20" s="41"/>
-    </row>
-    <row r="21" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C21" s="28"/>
-      <c r="D21" s="29"/>
-      <c r="E21" s="29"/>
-      <c r="F21" s="39"/>
-      <c r="G21" s="39"/>
-      <c r="H21" s="39"/>
-      <c r="I21" s="39"/>
-      <c r="J21" s="42"/>
-      <c r="L21" s="43"/>
-    </row>
-    <row r="22" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C22" s="14"/>
-      <c r="J22" s="13"/>
-      <c r="L22" s="43"/>
-    </row>
-    <row r="23" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C23" s="44" t="s">
-        <v>21</v>
-      </c>
-      <c r="D23" s="45"/>
-      <c r="E23" s="46"/>
-      <c r="F23" s="46"/>
-      <c r="G23" s="46"/>
-      <c r="H23" s="46"/>
-      <c r="I23" s="46"/>
-      <c r="J23" s="47"/>
-      <c r="L23" s="43"/>
-    </row>
-    <row r="24" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C24" s="14"/>
-      <c r="J24" s="13"/>
-      <c r="L24" s="43"/>
-    </row>
-    <row r="25" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C25" s="15" t="s">
-        <v>22</v>
-      </c>
-      <c r="D25" s="16"/>
-      <c r="E25" s="16"/>
+      <c r="D25" s="34"/>
+      <c r="E25" s="34"/>
       <c r="F25" s="35" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="G25" s="36"/>
       <c r="H25" s="36"/>
       <c r="I25" s="37"/>
-      <c r="J25" s="13"/>
-      <c r="L25" s="43"/>
-    </row>
-    <row r="26" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C26" s="28"/>
-      <c r="D26" s="29"/>
-      <c r="E26" s="29"/>
-      <c r="F26" s="34"/>
-      <c r="G26" s="34"/>
-      <c r="H26" s="34"/>
-      <c r="I26" s="34"/>
-      <c r="J26" s="13"/>
-      <c r="L26" s="43"/>
-    </row>
-    <row r="27" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C27" s="28"/>
-      <c r="D27" s="29"/>
-      <c r="E27" s="29"/>
-      <c r="F27" s="35" t="s">
-        <v>24</v>
-      </c>
-      <c r="G27" s="36"/>
-      <c r="H27" s="36"/>
-      <c r="I27" s="37"/>
-      <c r="J27" s="13"/>
-      <c r="L27" s="43"/>
-    </row>
-    <row r="28" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C28" s="28"/>
-      <c r="D28" s="29"/>
-      <c r="E28" s="29"/>
-      <c r="F28" s="34"/>
-      <c r="G28" s="34"/>
-      <c r="H28" s="34"/>
-      <c r="I28" s="34"/>
-      <c r="J28" s="13"/>
-      <c r="L28" s="43"/>
-    </row>
-    <row r="29" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C29" s="28"/>
-      <c r="D29" s="29"/>
-      <c r="E29" s="29"/>
-      <c r="J29" s="13"/>
-      <c r="L29" s="43"/>
-    </row>
-    <row r="30" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C30" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="D30" s="16"/>
-      <c r="E30" s="16"/>
+      <c r="J25" s="7"/>
+      <c r="L25" s="21"/>
+    </row>
+    <row r="26" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C26" s="9"/>
+      <c r="D26" s="10"/>
+      <c r="E26" s="10"/>
+      <c r="F26" s="11"/>
+      <c r="G26" s="11"/>
+      <c r="H26" s="11"/>
+      <c r="I26" s="11"/>
+      <c r="J26" s="7"/>
+      <c r="L26" s="21"/>
+    </row>
+    <row r="27" spans="3:12" ht="30.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C27" s="9"/>
+      <c r="D27" s="10"/>
+      <c r="E27" s="10"/>
+      <c r="F27" s="56" t="s">
+        <v>28</v>
+      </c>
+      <c r="G27" s="57"/>
+      <c r="H27" s="57"/>
+      <c r="I27" s="58"/>
+      <c r="J27" s="7"/>
+      <c r="L27" s="21"/>
+    </row>
+    <row r="28" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C28" s="9"/>
+      <c r="D28" s="10"/>
+      <c r="E28" s="10"/>
+      <c r="F28" s="11"/>
+      <c r="G28" s="11"/>
+      <c r="H28" s="11"/>
+      <c r="I28" s="11"/>
+      <c r="J28" s="7"/>
+      <c r="L28" s="21"/>
+    </row>
+    <row r="29" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C29" s="9"/>
+      <c r="D29" s="10"/>
+      <c r="E29" s="10"/>
+      <c r="J29" s="7"/>
+      <c r="L29" s="21"/>
+    </row>
+    <row r="30" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C30" s="33" t="s">
+        <v>16</v>
+      </c>
+      <c r="D30" s="34"/>
+      <c r="E30" s="34"/>
       <c r="F30" s="35" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="G30" s="36"/>
       <c r="H30" s="36"/>
       <c r="I30" s="37"/>
-      <c r="J30" s="13"/>
-      <c r="L30" s="43"/>
-    </row>
-    <row r="31" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C31" s="28"/>
-      <c r="D31" s="29"/>
-      <c r="E31" s="29"/>
-      <c r="F31" s="34"/>
-      <c r="G31" s="34"/>
-      <c r="H31" s="34"/>
-      <c r="I31" s="34"/>
-      <c r="J31" s="13"/>
-      <c r="L31" s="43"/>
-    </row>
-    <row r="32" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C32" s="28"/>
-      <c r="D32" s="29"/>
-      <c r="E32" s="29"/>
-      <c r="F32" s="35" t="s">
+      <c r="J30" s="7"/>
+      <c r="L30" s="21"/>
+    </row>
+    <row r="31" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C31" s="9"/>
+      <c r="D31" s="10"/>
+      <c r="E31" s="10"/>
+      <c r="F31" s="11"/>
+      <c r="G31" s="11"/>
+      <c r="H31" s="11"/>
+      <c r="I31" s="11"/>
+      <c r="J31" s="7"/>
+      <c r="L31" s="21"/>
+    </row>
+    <row r="32" spans="3:12" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C32" s="9"/>
+      <c r="D32" s="10"/>
+      <c r="E32" s="10"/>
+      <c r="F32" s="56" t="s">
+        <v>30</v>
+      </c>
+      <c r="G32" s="57"/>
+      <c r="H32" s="57"/>
+      <c r="I32" s="58"/>
+      <c r="J32" s="7"/>
+      <c r="L32" s="21"/>
+    </row>
+    <row r="33" spans="3:16" x14ac:dyDescent="0.3">
+      <c r="C33" s="9"/>
+      <c r="D33" s="10"/>
+      <c r="E33" s="10"/>
+      <c r="F33" s="11"/>
+      <c r="G33" s="11"/>
+      <c r="H33" s="11"/>
+      <c r="I33" s="11"/>
+      <c r="J33" s="7"/>
+      <c r="L33" s="21"/>
+    </row>
+    <row r="34" spans="3:16" x14ac:dyDescent="0.3">
+      <c r="C34" s="8"/>
+      <c r="J34" s="7"/>
+      <c r="L34" s="21"/>
+    </row>
+    <row r="35" spans="3:16" x14ac:dyDescent="0.3">
+      <c r="C35" s="33" t="s">
+        <v>17</v>
+      </c>
+      <c r="D35" s="34"/>
+      <c r="E35" s="34"/>
+      <c r="F35" s="35" t="s">
         <v>26</v>
-      </c>
-      <c r="G32" s="36"/>
-      <c r="H32" s="36"/>
-      <c r="I32" s="37"/>
-      <c r="J32" s="13"/>
-      <c r="L32" s="43"/>
-    </row>
-    <row r="33" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="C33" s="28"/>
-      <c r="D33" s="29"/>
-      <c r="E33" s="29"/>
-      <c r="F33" s="34"/>
-      <c r="G33" s="34"/>
-      <c r="H33" s="34"/>
-      <c r="I33" s="34"/>
-      <c r="J33" s="13"/>
-      <c r="L33" s="43"/>
-    </row>
-    <row r="34" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="C34" s="14"/>
-      <c r="J34" s="13"/>
-      <c r="L34" s="43"/>
-    </row>
-    <row r="35" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="C35" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="D35" s="16"/>
-      <c r="E35" s="16"/>
-      <c r="F35" s="35" t="s">
-        <v>28</v>
       </c>
       <c r="G35" s="36"/>
       <c r="H35" s="36"/>
       <c r="I35" s="37"/>
-      <c r="J35" s="13"/>
-      <c r="L35" s="43"/>
-    </row>
-    <row r="36" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="C36" s="28"/>
-      <c r="D36" s="29"/>
-      <c r="E36" s="29"/>
-      <c r="J36" s="13"/>
-      <c r="L36" s="43"/>
-    </row>
-    <row r="37" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="C37" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="D37" s="16"/>
-      <c r="E37" s="16"/>
+      <c r="J35" s="7"/>
+      <c r="L35" s="21"/>
+    </row>
+    <row r="36" spans="3:16" x14ac:dyDescent="0.3">
+      <c r="C36" s="9"/>
+      <c r="D36" s="10"/>
+      <c r="E36" s="10"/>
+      <c r="J36" s="7"/>
+      <c r="L36" s="21"/>
+    </row>
+    <row r="37" spans="3:16" x14ac:dyDescent="0.3">
+      <c r="C37" s="33" t="s">
+        <v>18</v>
+      </c>
+      <c r="D37" s="34"/>
+      <c r="E37" s="34"/>
       <c r="F37" s="35" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="G37" s="36"/>
       <c r="H37" s="36"/>
       <c r="I37" s="37"/>
-      <c r="J37" s="13"/>
-      <c r="L37" s="43"/>
-    </row>
-    <row r="38" spans="3:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C38" s="48"/>
-      <c r="D38" s="49"/>
-      <c r="E38" s="49"/>
-      <c r="F38" s="49"/>
-      <c r="G38" s="49"/>
-      <c r="H38" s="49"/>
-      <c r="I38" s="49"/>
-      <c r="J38" s="50"/>
-      <c r="L38" s="43"/>
-    </row>
-    <row r="39" spans="3:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C39" s="51" t="s">
-        <v>31</v>
-      </c>
-      <c r="D39" s="52"/>
-      <c r="E39" s="52"/>
-      <c r="F39" s="52"/>
-      <c r="G39" s="52"/>
-      <c r="H39" s="52"/>
-      <c r="I39" s="53" t="s">
-        <v>32</v>
-      </c>
-      <c r="J39" s="54"/>
-      <c r="L39" s="43"/>
-    </row>
-    <row r="40" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="L40" s="55"/>
-    </row>
-    <row r="46" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="P46" s="56"/>
+      <c r="J37" s="7"/>
+      <c r="L37" s="21"/>
+    </row>
+    <row r="38" spans="3:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C38" s="24"/>
+      <c r="D38" s="25"/>
+      <c r="E38" s="25"/>
+      <c r="F38" s="25"/>
+      <c r="G38" s="25"/>
+      <c r="H38" s="25"/>
+      <c r="I38" s="25"/>
+      <c r="J38" s="26"/>
+      <c r="L38" s="21"/>
+    </row>
+    <row r="39" spans="3:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C39" s="29" t="s">
+        <v>19</v>
+      </c>
+      <c r="D39" s="30"/>
+      <c r="E39" s="30"/>
+      <c r="F39" s="30"/>
+      <c r="G39" s="30"/>
+      <c r="H39" s="30"/>
+      <c r="I39" s="31" t="s">
+        <v>20</v>
+      </c>
+      <c r="J39" s="32"/>
+      <c r="L39" s="21"/>
+    </row>
+    <row r="40" spans="3:16" x14ac:dyDescent="0.3">
+      <c r="L40" s="27"/>
+    </row>
+    <row r="46" spans="3:16" x14ac:dyDescent="0.3">
+      <c r="P46" s="28"/>
     </row>
   </sheetData>
   <mergeCells count="29">
+    <mergeCell ref="C8:E8"/>
+    <mergeCell ref="F8:I8"/>
+    <mergeCell ref="C4:F4"/>
+    <mergeCell ref="G4:J4"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="C7:E7"/>
+    <mergeCell ref="F7:I7"/>
+    <mergeCell ref="F27:I27"/>
+    <mergeCell ref="C9:E9"/>
+    <mergeCell ref="F9:I9"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="C13:E13"/>
+    <mergeCell ref="F13:I14"/>
+    <mergeCell ref="C16:E16"/>
+    <mergeCell ref="F16:I16"/>
+    <mergeCell ref="F18:I18"/>
+    <mergeCell ref="F20:I21"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="C25:E25"/>
+    <mergeCell ref="F25:I25"/>
     <mergeCell ref="C39:H39"/>
     <mergeCell ref="I39:J39"/>
     <mergeCell ref="C30:E30"/>
@@ -1514,27 +1559,10 @@
     <mergeCell ref="F35:I35"/>
     <mergeCell ref="C37:E37"/>
     <mergeCell ref="F37:I37"/>
-    <mergeCell ref="F18:I18"/>
-    <mergeCell ref="F20:I21"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="C25:E25"/>
-    <mergeCell ref="F25:I25"/>
-    <mergeCell ref="F27:I27"/>
-    <mergeCell ref="C9:E9"/>
-    <mergeCell ref="F9:I9"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="C13:E13"/>
-    <mergeCell ref="F13:I14"/>
-    <mergeCell ref="C16:E16"/>
-    <mergeCell ref="F16:I16"/>
-    <mergeCell ref="C4:F4"/>
-    <mergeCell ref="G4:J4"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="C7:E7"/>
-    <mergeCell ref="F7:I7"/>
-    <mergeCell ref="C8:E8"/>
-    <mergeCell ref="F8:I8"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="F8" r:id="rId1" xr:uid="{24426368-5A6C-4187-9C63-3E3C53FC250F}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
 </worksheet>

</xml_diff>

<commit_message>
Información actualizada - NBQ050100
</commit_message>
<xml_diff>
--- a/ControlCambios/05_Planificacion/Plan_001.xlsx
+++ b/ControlCambios/05_Planificacion/Plan_001.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Niko\Documents\Uni\EnSo\EnSo_ControlCambios_gr1.2\ControlCambios\05_Planificacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D29C2312-1EC8-4351-991C-380F62AE2D0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{935E0BB7-BB2C-4407-B0DD-8302AF1C3D0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{A0B7CE81-5765-4616-ABB9-45231285591F}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{A0B7CE81-5765-4616-ABB9-45231285591F}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan" sheetId="1" r:id="rId1"/>
@@ -110,9 +110,6 @@
     <t>NBQ_050100</t>
   </si>
   <si>
-    <t>1 semana</t>
-  </si>
-  <si>
     <t>Gerente del proyecto, equipo de desarrollo</t>
   </si>
   <si>
@@ -138,6 +135,9 @@
   </si>
   <si>
     <t>7.33 días</t>
+  </si>
+  <si>
+    <t>3 días</t>
   </si>
 </sst>
 </file>
@@ -693,31 +693,70 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="7" fillId="2" borderId="32" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -729,65 +768,26 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="7" fillId="2" borderId="32" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1107,7 +1107,7 @@
   <dimension ref="C2:P46"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F38" sqref="F38"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1132,24 +1132,24 @@
       <c r="J3" s="6"/>
     </row>
     <row r="4" spans="3:13" x14ac:dyDescent="0.3">
-      <c r="C4" s="50" t="s">
+      <c r="C4" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="51"/>
-      <c r="E4" s="51"/>
-      <c r="F4" s="51"/>
-      <c r="G4" s="52" t="s">
+      <c r="D4" s="34"/>
+      <c r="E4" s="34"/>
+      <c r="F4" s="34"/>
+      <c r="G4" s="35" t="s">
         <v>4</v>
       </c>
-      <c r="H4" s="52"/>
-      <c r="I4" s="52"/>
-      <c r="J4" s="53"/>
+      <c r="H4" s="35"/>
+      <c r="I4" s="35"/>
+      <c r="J4" s="36"/>
     </row>
     <row r="5" spans="3:13" x14ac:dyDescent="0.3">
-      <c r="C5" s="43" t="s">
+      <c r="C5" s="37" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="44"/>
+      <c r="D5" s="38"/>
       <c r="J5" s="7"/>
     </row>
     <row r="6" spans="3:13" x14ac:dyDescent="0.3">
@@ -1157,45 +1157,45 @@
       <c r="J6" s="7"/>
     </row>
     <row r="7" spans="3:13" x14ac:dyDescent="0.3">
-      <c r="C7" s="33" t="s">
+      <c r="C7" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="34"/>
-      <c r="E7" s="34"/>
-      <c r="F7" s="54" t="s">
+      <c r="D7" s="30"/>
+      <c r="E7" s="30"/>
+      <c r="F7" s="32" t="s">
         <v>21</v>
       </c>
-      <c r="G7" s="54"/>
-      <c r="H7" s="54"/>
-      <c r="I7" s="54"/>
+      <c r="G7" s="32"/>
+      <c r="H7" s="32"/>
+      <c r="I7" s="32"/>
       <c r="J7" s="7"/>
     </row>
     <row r="8" spans="3:13" x14ac:dyDescent="0.3">
-      <c r="C8" s="33" t="s">
+      <c r="C8" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="D8" s="34"/>
-      <c r="E8" s="34"/>
-      <c r="F8" s="55" t="s">
+      <c r="D8" s="30"/>
+      <c r="E8" s="30"/>
+      <c r="F8" s="31" t="s">
         <v>22</v>
       </c>
-      <c r="G8" s="54"/>
-      <c r="H8" s="54"/>
-      <c r="I8" s="54"/>
+      <c r="G8" s="32"/>
+      <c r="H8" s="32"/>
+      <c r="I8" s="32"/>
       <c r="J8" s="7"/>
     </row>
     <row r="9" spans="3:13" x14ac:dyDescent="0.3">
-      <c r="C9" s="33" t="s">
+      <c r="C9" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="D9" s="34"/>
-      <c r="E9" s="34"/>
-      <c r="F9" s="41" t="s">
+      <c r="D9" s="30"/>
+      <c r="E9" s="30"/>
+      <c r="F9" s="42" t="s">
         <v>23</v>
       </c>
-      <c r="G9" s="42"/>
-      <c r="H9" s="42"/>
-      <c r="I9" s="42"/>
+      <c r="G9" s="43"/>
+      <c r="H9" s="43"/>
+      <c r="I9" s="43"/>
       <c r="J9" s="7"/>
     </row>
     <row r="10" spans="3:13" ht="15.6" x14ac:dyDescent="0.3">
@@ -1210,10 +1210,10 @@
       <c r="M10" s="15"/>
     </row>
     <row r="11" spans="3:13" x14ac:dyDescent="0.3">
-      <c r="C11" s="43" t="s">
+      <c r="C11" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="D11" s="44"/>
+      <c r="D11" s="38"/>
       <c r="J11" s="7"/>
     </row>
     <row r="12" spans="3:13" x14ac:dyDescent="0.3">
@@ -1221,27 +1221,27 @@
       <c r="J12" s="7"/>
     </row>
     <row r="13" spans="3:13" x14ac:dyDescent="0.3">
-      <c r="C13" s="33" t="s">
+      <c r="C13" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="D13" s="34"/>
-      <c r="E13" s="45"/>
-      <c r="F13" s="59" t="s">
-        <v>24</v>
-      </c>
-      <c r="G13" s="60"/>
-      <c r="H13" s="60"/>
-      <c r="I13" s="60"/>
+      <c r="D13" s="30"/>
+      <c r="E13" s="44"/>
+      <c r="F13" s="45" t="s">
+        <v>33</v>
+      </c>
+      <c r="G13" s="46"/>
+      <c r="H13" s="46"/>
+      <c r="I13" s="46"/>
       <c r="J13" s="16"/>
     </row>
     <row r="14" spans="3:13" x14ac:dyDescent="0.3">
       <c r="C14" s="9"/>
       <c r="D14" s="10"/>
       <c r="E14" s="10"/>
-      <c r="F14" s="60"/>
-      <c r="G14" s="60"/>
-      <c r="H14" s="60"/>
-      <c r="I14" s="60"/>
+      <c r="F14" s="46"/>
+      <c r="G14" s="46"/>
+      <c r="H14" s="46"/>
+      <c r="I14" s="46"/>
       <c r="J14" s="16"/>
     </row>
     <row r="15" spans="3:13" x14ac:dyDescent="0.3">
@@ -1251,17 +1251,17 @@
       <c r="J15" s="7"/>
     </row>
     <row r="16" spans="3:13" x14ac:dyDescent="0.3">
-      <c r="C16" s="33" t="s">
+      <c r="C16" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="D16" s="34"/>
-      <c r="E16" s="46"/>
-      <c r="F16" s="47" t="s">
-        <v>25</v>
-      </c>
-      <c r="G16" s="48"/>
-      <c r="H16" s="48"/>
-      <c r="I16" s="49"/>
+      <c r="D16" s="30"/>
+      <c r="E16" s="47"/>
+      <c r="F16" s="48" t="s">
+        <v>24</v>
+      </c>
+      <c r="G16" s="49"/>
+      <c r="H16" s="49"/>
+      <c r="I16" s="50"/>
       <c r="J16" s="7"/>
     </row>
     <row r="17" spans="3:12" x14ac:dyDescent="0.3">
@@ -1280,12 +1280,12 @@
         <v>12</v>
       </c>
       <c r="E18" s="10"/>
-      <c r="F18" s="56" t="s">
-        <v>31</v>
-      </c>
-      <c r="G18" s="57"/>
-      <c r="H18" s="57"/>
-      <c r="I18" s="58"/>
+      <c r="F18" s="39" t="s">
+        <v>30</v>
+      </c>
+      <c r="G18" s="40"/>
+      <c r="H18" s="40"/>
+      <c r="I18" s="41"/>
       <c r="J18" s="7"/>
     </row>
     <row r="19" spans="3:12" x14ac:dyDescent="0.3">
@@ -1304,12 +1304,12 @@
         <v>13</v>
       </c>
       <c r="E20" s="10"/>
-      <c r="F20" s="38" t="s">
-        <v>32</v>
-      </c>
-      <c r="G20" s="38"/>
-      <c r="H20" s="38"/>
-      <c r="I20" s="38"/>
+      <c r="F20" s="51" t="s">
+        <v>31</v>
+      </c>
+      <c r="G20" s="51"/>
+      <c r="H20" s="51"/>
+      <c r="I20" s="51"/>
       <c r="J20" s="18"/>
       <c r="L20" s="19"/>
     </row>
@@ -1317,10 +1317,10 @@
       <c r="C21" s="9"/>
       <c r="D21" s="10"/>
       <c r="E21" s="10"/>
-      <c r="F21" s="38"/>
-      <c r="G21" s="38"/>
-      <c r="H21" s="38"/>
-      <c r="I21" s="38"/>
+      <c r="F21" s="51"/>
+      <c r="G21" s="51"/>
+      <c r="H21" s="51"/>
+      <c r="I21" s="51"/>
       <c r="J21" s="20"/>
       <c r="L21" s="21"/>
     </row>
@@ -1330,10 +1330,10 @@
       <c r="L22" s="21"/>
     </row>
     <row r="23" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C23" s="39" t="s">
+      <c r="C23" s="52" t="s">
         <v>14</v>
       </c>
-      <c r="D23" s="40"/>
+      <c r="D23" s="53"/>
       <c r="E23" s="22"/>
       <c r="F23" s="22"/>
       <c r="G23" s="22"/>
@@ -1348,17 +1348,17 @@
       <c r="L24" s="21"/>
     </row>
     <row r="25" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C25" s="33" t="s">
+      <c r="C25" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="D25" s="34"/>
-      <c r="E25" s="34"/>
-      <c r="F25" s="35" t="s">
-        <v>27</v>
-      </c>
-      <c r="G25" s="36"/>
-      <c r="H25" s="36"/>
-      <c r="I25" s="37"/>
+      <c r="D25" s="30"/>
+      <c r="E25" s="30"/>
+      <c r="F25" s="54" t="s">
+        <v>26</v>
+      </c>
+      <c r="G25" s="55"/>
+      <c r="H25" s="55"/>
+      <c r="I25" s="56"/>
       <c r="J25" s="7"/>
       <c r="L25" s="21"/>
     </row>
@@ -1377,12 +1377,12 @@
       <c r="C27" s="9"/>
       <c r="D27" s="10"/>
       <c r="E27" s="10"/>
-      <c r="F27" s="56" t="s">
-        <v>28</v>
-      </c>
-      <c r="G27" s="57"/>
-      <c r="H27" s="57"/>
-      <c r="I27" s="58"/>
+      <c r="F27" s="39" t="s">
+        <v>27</v>
+      </c>
+      <c r="G27" s="40"/>
+      <c r="H27" s="40"/>
+      <c r="I27" s="41"/>
       <c r="J27" s="7"/>
       <c r="L27" s="21"/>
     </row>
@@ -1405,17 +1405,17 @@
       <c r="L29" s="21"/>
     </row>
     <row r="30" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C30" s="33" t="s">
+      <c r="C30" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="D30" s="34"/>
-      <c r="E30" s="34"/>
-      <c r="F30" s="35" t="s">
-        <v>29</v>
-      </c>
-      <c r="G30" s="36"/>
-      <c r="H30" s="36"/>
-      <c r="I30" s="37"/>
+      <c r="D30" s="30"/>
+      <c r="E30" s="30"/>
+      <c r="F30" s="54" t="s">
+        <v>28</v>
+      </c>
+      <c r="G30" s="55"/>
+      <c r="H30" s="55"/>
+      <c r="I30" s="56"/>
       <c r="J30" s="7"/>
       <c r="L30" s="21"/>
     </row>
@@ -1434,12 +1434,12 @@
       <c r="C32" s="9"/>
       <c r="D32" s="10"/>
       <c r="E32" s="10"/>
-      <c r="F32" s="56" t="s">
-        <v>30</v>
-      </c>
-      <c r="G32" s="57"/>
-      <c r="H32" s="57"/>
-      <c r="I32" s="58"/>
+      <c r="F32" s="39" t="s">
+        <v>29</v>
+      </c>
+      <c r="G32" s="40"/>
+      <c r="H32" s="40"/>
+      <c r="I32" s="41"/>
       <c r="J32" s="7"/>
       <c r="L32" s="21"/>
     </row>
@@ -1460,17 +1460,17 @@
       <c r="L34" s="21"/>
     </row>
     <row r="35" spans="3:16" x14ac:dyDescent="0.3">
-      <c r="C35" s="33" t="s">
+      <c r="C35" s="29" t="s">
         <v>17</v>
       </c>
-      <c r="D35" s="34"/>
-      <c r="E35" s="34"/>
-      <c r="F35" s="35" t="s">
-        <v>26</v>
-      </c>
-      <c r="G35" s="36"/>
-      <c r="H35" s="36"/>
-      <c r="I35" s="37"/>
+      <c r="D35" s="30"/>
+      <c r="E35" s="30"/>
+      <c r="F35" s="54" t="s">
+        <v>25</v>
+      </c>
+      <c r="G35" s="55"/>
+      <c r="H35" s="55"/>
+      <c r="I35" s="56"/>
       <c r="J35" s="7"/>
       <c r="L35" s="21"/>
     </row>
@@ -1482,17 +1482,17 @@
       <c r="L36" s="21"/>
     </row>
     <row r="37" spans="3:16" x14ac:dyDescent="0.3">
-      <c r="C37" s="33" t="s">
+      <c r="C37" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="D37" s="34"/>
-      <c r="E37" s="34"/>
-      <c r="F37" s="35" t="s">
-        <v>33</v>
-      </c>
-      <c r="G37" s="36"/>
-      <c r="H37" s="36"/>
-      <c r="I37" s="37"/>
+      <c r="D37" s="30"/>
+      <c r="E37" s="30"/>
+      <c r="F37" s="54" t="s">
+        <v>32</v>
+      </c>
+      <c r="G37" s="55"/>
+      <c r="H37" s="55"/>
+      <c r="I37" s="56"/>
       <c r="J37" s="7"/>
       <c r="L37" s="21"/>
     </row>
@@ -1508,18 +1508,18 @@
       <c r="L38" s="21"/>
     </row>
     <row r="39" spans="3:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C39" s="29" t="s">
+      <c r="C39" s="57" t="s">
         <v>19</v>
       </c>
-      <c r="D39" s="30"/>
-      <c r="E39" s="30"/>
-      <c r="F39" s="30"/>
-      <c r="G39" s="30"/>
-      <c r="H39" s="30"/>
-      <c r="I39" s="31" t="s">
+      <c r="D39" s="58"/>
+      <c r="E39" s="58"/>
+      <c r="F39" s="58"/>
+      <c r="G39" s="58"/>
+      <c r="H39" s="58"/>
+      <c r="I39" s="59" t="s">
         <v>20</v>
       </c>
-      <c r="J39" s="32"/>
+      <c r="J39" s="60"/>
       <c r="L39" s="21"/>
     </row>
     <row r="40" spans="3:16" x14ac:dyDescent="0.3">
@@ -1530,13 +1530,15 @@
     </row>
   </sheetData>
   <mergeCells count="29">
-    <mergeCell ref="C8:E8"/>
-    <mergeCell ref="F8:I8"/>
-    <mergeCell ref="C4:F4"/>
-    <mergeCell ref="G4:J4"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="C7:E7"/>
-    <mergeCell ref="F7:I7"/>
+    <mergeCell ref="C39:H39"/>
+    <mergeCell ref="I39:J39"/>
+    <mergeCell ref="C30:E30"/>
+    <mergeCell ref="F30:I30"/>
+    <mergeCell ref="F32:I32"/>
+    <mergeCell ref="C35:E35"/>
+    <mergeCell ref="F35:I35"/>
+    <mergeCell ref="C37:E37"/>
+    <mergeCell ref="F37:I37"/>
     <mergeCell ref="F27:I27"/>
     <mergeCell ref="C9:E9"/>
     <mergeCell ref="F9:I9"/>
@@ -1550,15 +1552,13 @@
     <mergeCell ref="C23:D23"/>
     <mergeCell ref="C25:E25"/>
     <mergeCell ref="F25:I25"/>
-    <mergeCell ref="C39:H39"/>
-    <mergeCell ref="I39:J39"/>
-    <mergeCell ref="C30:E30"/>
-    <mergeCell ref="F30:I30"/>
-    <mergeCell ref="F32:I32"/>
-    <mergeCell ref="C35:E35"/>
-    <mergeCell ref="F35:I35"/>
-    <mergeCell ref="C37:E37"/>
-    <mergeCell ref="F37:I37"/>
+    <mergeCell ref="C8:E8"/>
+    <mergeCell ref="F8:I8"/>
+    <mergeCell ref="C4:F4"/>
+    <mergeCell ref="G4:J4"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="C7:E7"/>
+    <mergeCell ref="F7:I7"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="F8" r:id="rId1" xr:uid="{24426368-5A6C-4187-9C63-3E3C53FC250F}"/>

</xml_diff>

<commit_message>
Decimales eliminados - NBQ_050100
</commit_message>
<xml_diff>
--- a/ControlCambios/05_Planificacion/Plan_001.xlsx
+++ b/ControlCambios/05_Planificacion/Plan_001.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Niko\Documents\Uni\EnSo\EnSo_ControlCambios_gr1.2\ControlCambios\05_Planificacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{935E0BB7-BB2C-4407-B0DD-8302AF1C3D0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0825EE8-4CC7-4C8E-B267-5FAE7C98DBAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{A0B7CE81-5765-4616-ABB9-45231285591F}"/>
   </bookViews>
@@ -134,10 +134,10 @@
     <t xml:space="preserve">Implementar medidas para el manejo de grandes volúmenes de datos, colaborar con expertos en múltiples sistemas operativos. </t>
   </si>
   <si>
-    <t>7.33 días</t>
-  </si>
-  <si>
     <t>3 días</t>
+  </si>
+  <si>
+    <t>7 días</t>
   </si>
 </sst>
 </file>
@@ -693,10 +693,82 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="7" fillId="2" borderId="32" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyAlignment="1">
@@ -716,78 +788,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="7" fillId="2" borderId="32" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1106,8 +1106,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50348CFE-78AC-4183-AE37-6C1BCA731247}">
   <dimension ref="C2:P46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView tabSelected="1" topLeftCell="B22" workbookViewId="0">
+      <selection activeCell="M28" sqref="M28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1132,24 +1132,24 @@
       <c r="J3" s="6"/>
     </row>
     <row r="4" spans="3:13" x14ac:dyDescent="0.3">
-      <c r="C4" s="33" t="s">
+      <c r="C4" s="57" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="34"/>
-      <c r="E4" s="34"/>
-      <c r="F4" s="34"/>
-      <c r="G4" s="35" t="s">
+      <c r="D4" s="58"/>
+      <c r="E4" s="58"/>
+      <c r="F4" s="58"/>
+      <c r="G4" s="59" t="s">
         <v>4</v>
       </c>
-      <c r="H4" s="35"/>
-      <c r="I4" s="35"/>
-      <c r="J4" s="36"/>
+      <c r="H4" s="59"/>
+      <c r="I4" s="59"/>
+      <c r="J4" s="60"/>
     </row>
     <row r="5" spans="3:13" x14ac:dyDescent="0.3">
-      <c r="C5" s="37" t="s">
+      <c r="C5" s="43" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="38"/>
+      <c r="D5" s="44"/>
       <c r="J5" s="7"/>
     </row>
     <row r="6" spans="3:13" x14ac:dyDescent="0.3">
@@ -1157,45 +1157,45 @@
       <c r="J6" s="7"/>
     </row>
     <row r="7" spans="3:13" x14ac:dyDescent="0.3">
-      <c r="C7" s="29" t="s">
+      <c r="C7" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="30"/>
-      <c r="E7" s="30"/>
-      <c r="F7" s="32" t="s">
+      <c r="D7" s="34"/>
+      <c r="E7" s="34"/>
+      <c r="F7" s="56" t="s">
         <v>21</v>
       </c>
-      <c r="G7" s="32"/>
-      <c r="H7" s="32"/>
-      <c r="I7" s="32"/>
+      <c r="G7" s="56"/>
+      <c r="H7" s="56"/>
+      <c r="I7" s="56"/>
       <c r="J7" s="7"/>
     </row>
     <row r="8" spans="3:13" x14ac:dyDescent="0.3">
-      <c r="C8" s="29" t="s">
+      <c r="C8" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="D8" s="30"/>
-      <c r="E8" s="30"/>
-      <c r="F8" s="31" t="s">
+      <c r="D8" s="34"/>
+      <c r="E8" s="34"/>
+      <c r="F8" s="55" t="s">
         <v>22</v>
       </c>
-      <c r="G8" s="32"/>
-      <c r="H8" s="32"/>
-      <c r="I8" s="32"/>
+      <c r="G8" s="56"/>
+      <c r="H8" s="56"/>
+      <c r="I8" s="56"/>
       <c r="J8" s="7"/>
     </row>
     <row r="9" spans="3:13" x14ac:dyDescent="0.3">
-      <c r="C9" s="29" t="s">
+      <c r="C9" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="D9" s="30"/>
-      <c r="E9" s="30"/>
-      <c r="F9" s="42" t="s">
+      <c r="D9" s="34"/>
+      <c r="E9" s="34"/>
+      <c r="F9" s="41" t="s">
         <v>23</v>
       </c>
-      <c r="G9" s="43"/>
-      <c r="H9" s="43"/>
-      <c r="I9" s="43"/>
+      <c r="G9" s="42"/>
+      <c r="H9" s="42"/>
+      <c r="I9" s="42"/>
       <c r="J9" s="7"/>
     </row>
     <row r="10" spans="3:13" ht="15.6" x14ac:dyDescent="0.3">
@@ -1210,10 +1210,10 @@
       <c r="M10" s="15"/>
     </row>
     <row r="11" spans="3:13" x14ac:dyDescent="0.3">
-      <c r="C11" s="37" t="s">
+      <c r="C11" s="43" t="s">
         <v>9</v>
       </c>
-      <c r="D11" s="38"/>
+      <c r="D11" s="44"/>
       <c r="J11" s="7"/>
     </row>
     <row r="12" spans="3:13" x14ac:dyDescent="0.3">
@@ -1221,27 +1221,27 @@
       <c r="J12" s="7"/>
     </row>
     <row r="13" spans="3:13" x14ac:dyDescent="0.3">
-      <c r="C13" s="29" t="s">
+      <c r="C13" s="33" t="s">
         <v>10</v>
       </c>
-      <c r="D13" s="30"/>
-      <c r="E13" s="44"/>
-      <c r="F13" s="45" t="s">
-        <v>33</v>
-      </c>
-      <c r="G13" s="46"/>
-      <c r="H13" s="46"/>
-      <c r="I13" s="46"/>
+      <c r="D13" s="34"/>
+      <c r="E13" s="45"/>
+      <c r="F13" s="46" t="s">
+        <v>32</v>
+      </c>
+      <c r="G13" s="47"/>
+      <c r="H13" s="47"/>
+      <c r="I13" s="47"/>
       <c r="J13" s="16"/>
     </row>
     <row r="14" spans="3:13" x14ac:dyDescent="0.3">
       <c r="C14" s="9"/>
       <c r="D14" s="10"/>
       <c r="E14" s="10"/>
-      <c r="F14" s="46"/>
-      <c r="G14" s="46"/>
-      <c r="H14" s="46"/>
-      <c r="I14" s="46"/>
+      <c r="F14" s="47"/>
+      <c r="G14" s="47"/>
+      <c r="H14" s="47"/>
+      <c r="I14" s="47"/>
       <c r="J14" s="16"/>
     </row>
     <row r="15" spans="3:13" x14ac:dyDescent="0.3">
@@ -1251,17 +1251,17 @@
       <c r="J15" s="7"/>
     </row>
     <row r="16" spans="3:13" x14ac:dyDescent="0.3">
-      <c r="C16" s="29" t="s">
+      <c r="C16" s="33" t="s">
         <v>11</v>
       </c>
-      <c r="D16" s="30"/>
-      <c r="E16" s="47"/>
-      <c r="F16" s="48" t="s">
+      <c r="D16" s="34"/>
+      <c r="E16" s="48"/>
+      <c r="F16" s="49" t="s">
         <v>24</v>
       </c>
-      <c r="G16" s="49"/>
-      <c r="H16" s="49"/>
-      <c r="I16" s="50"/>
+      <c r="G16" s="50"/>
+      <c r="H16" s="50"/>
+      <c r="I16" s="51"/>
       <c r="J16" s="7"/>
     </row>
     <row r="17" spans="3:12" x14ac:dyDescent="0.3">
@@ -1280,12 +1280,12 @@
         <v>12</v>
       </c>
       <c r="E18" s="10"/>
-      <c r="F18" s="39" t="s">
+      <c r="F18" s="38" t="s">
         <v>30</v>
       </c>
-      <c r="G18" s="40"/>
-      <c r="H18" s="40"/>
-      <c r="I18" s="41"/>
+      <c r="G18" s="39"/>
+      <c r="H18" s="39"/>
+      <c r="I18" s="40"/>
       <c r="J18" s="7"/>
     </row>
     <row r="19" spans="3:12" x14ac:dyDescent="0.3">
@@ -1304,12 +1304,12 @@
         <v>13</v>
       </c>
       <c r="E20" s="10"/>
-      <c r="F20" s="51" t="s">
+      <c r="F20" s="52" t="s">
         <v>31</v>
       </c>
-      <c r="G20" s="51"/>
-      <c r="H20" s="51"/>
-      <c r="I20" s="51"/>
+      <c r="G20" s="52"/>
+      <c r="H20" s="52"/>
+      <c r="I20" s="52"/>
       <c r="J20" s="18"/>
       <c r="L20" s="19"/>
     </row>
@@ -1317,10 +1317,10 @@
       <c r="C21" s="9"/>
       <c r="D21" s="10"/>
       <c r="E21" s="10"/>
-      <c r="F21" s="51"/>
-      <c r="G21" s="51"/>
-      <c r="H21" s="51"/>
-      <c r="I21" s="51"/>
+      <c r="F21" s="52"/>
+      <c r="G21" s="52"/>
+      <c r="H21" s="52"/>
+      <c r="I21" s="52"/>
       <c r="J21" s="20"/>
       <c r="L21" s="21"/>
     </row>
@@ -1330,10 +1330,10 @@
       <c r="L22" s="21"/>
     </row>
     <row r="23" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C23" s="52" t="s">
+      <c r="C23" s="53" t="s">
         <v>14</v>
       </c>
-      <c r="D23" s="53"/>
+      <c r="D23" s="54"/>
       <c r="E23" s="22"/>
       <c r="F23" s="22"/>
       <c r="G23" s="22"/>
@@ -1348,17 +1348,17 @@
       <c r="L24" s="21"/>
     </row>
     <row r="25" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C25" s="29" t="s">
+      <c r="C25" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="D25" s="30"/>
-      <c r="E25" s="30"/>
-      <c r="F25" s="54" t="s">
+      <c r="D25" s="34"/>
+      <c r="E25" s="34"/>
+      <c r="F25" s="35" t="s">
         <v>26</v>
       </c>
-      <c r="G25" s="55"/>
-      <c r="H25" s="55"/>
-      <c r="I25" s="56"/>
+      <c r="G25" s="36"/>
+      <c r="H25" s="36"/>
+      <c r="I25" s="37"/>
       <c r="J25" s="7"/>
       <c r="L25" s="21"/>
     </row>
@@ -1377,12 +1377,12 @@
       <c r="C27" s="9"/>
       <c r="D27" s="10"/>
       <c r="E27" s="10"/>
-      <c r="F27" s="39" t="s">
+      <c r="F27" s="38" t="s">
         <v>27</v>
       </c>
-      <c r="G27" s="40"/>
-      <c r="H27" s="40"/>
-      <c r="I27" s="41"/>
+      <c r="G27" s="39"/>
+      <c r="H27" s="39"/>
+      <c r="I27" s="40"/>
       <c r="J27" s="7"/>
       <c r="L27" s="21"/>
     </row>
@@ -1405,17 +1405,17 @@
       <c r="L29" s="21"/>
     </row>
     <row r="30" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C30" s="29" t="s">
+      <c r="C30" s="33" t="s">
         <v>16</v>
       </c>
-      <c r="D30" s="30"/>
-      <c r="E30" s="30"/>
-      <c r="F30" s="54" t="s">
+      <c r="D30" s="34"/>
+      <c r="E30" s="34"/>
+      <c r="F30" s="35" t="s">
         <v>28</v>
       </c>
-      <c r="G30" s="55"/>
-      <c r="H30" s="55"/>
-      <c r="I30" s="56"/>
+      <c r="G30" s="36"/>
+      <c r="H30" s="36"/>
+      <c r="I30" s="37"/>
       <c r="J30" s="7"/>
       <c r="L30" s="21"/>
     </row>
@@ -1434,12 +1434,12 @@
       <c r="C32" s="9"/>
       <c r="D32" s="10"/>
       <c r="E32" s="10"/>
-      <c r="F32" s="39" t="s">
+      <c r="F32" s="38" t="s">
         <v>29</v>
       </c>
-      <c r="G32" s="40"/>
-      <c r="H32" s="40"/>
-      <c r="I32" s="41"/>
+      <c r="G32" s="39"/>
+      <c r="H32" s="39"/>
+      <c r="I32" s="40"/>
       <c r="J32" s="7"/>
       <c r="L32" s="21"/>
     </row>
@@ -1460,17 +1460,17 @@
       <c r="L34" s="21"/>
     </row>
     <row r="35" spans="3:16" x14ac:dyDescent="0.3">
-      <c r="C35" s="29" t="s">
+      <c r="C35" s="33" t="s">
         <v>17</v>
       </c>
-      <c r="D35" s="30"/>
-      <c r="E35" s="30"/>
-      <c r="F35" s="54" t="s">
+      <c r="D35" s="34"/>
+      <c r="E35" s="34"/>
+      <c r="F35" s="35" t="s">
         <v>25</v>
       </c>
-      <c r="G35" s="55"/>
-      <c r="H35" s="55"/>
-      <c r="I35" s="56"/>
+      <c r="G35" s="36"/>
+      <c r="H35" s="36"/>
+      <c r="I35" s="37"/>
       <c r="J35" s="7"/>
       <c r="L35" s="21"/>
     </row>
@@ -1482,17 +1482,17 @@
       <c r="L36" s="21"/>
     </row>
     <row r="37" spans="3:16" x14ac:dyDescent="0.3">
-      <c r="C37" s="29" t="s">
+      <c r="C37" s="33" t="s">
         <v>18</v>
       </c>
-      <c r="D37" s="30"/>
-      <c r="E37" s="30"/>
-      <c r="F37" s="54" t="s">
-        <v>32</v>
-      </c>
-      <c r="G37" s="55"/>
-      <c r="H37" s="55"/>
-      <c r="I37" s="56"/>
+      <c r="D37" s="34"/>
+      <c r="E37" s="34"/>
+      <c r="F37" s="35" t="s">
+        <v>33</v>
+      </c>
+      <c r="G37" s="36"/>
+      <c r="H37" s="36"/>
+      <c r="I37" s="37"/>
       <c r="J37" s="7"/>
       <c r="L37" s="21"/>
     </row>
@@ -1508,18 +1508,18 @@
       <c r="L38" s="21"/>
     </row>
     <row r="39" spans="3:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C39" s="57" t="s">
+      <c r="C39" s="29" t="s">
         <v>19</v>
       </c>
-      <c r="D39" s="58"/>
-      <c r="E39" s="58"/>
-      <c r="F39" s="58"/>
-      <c r="G39" s="58"/>
-      <c r="H39" s="58"/>
-      <c r="I39" s="59" t="s">
+      <c r="D39" s="30"/>
+      <c r="E39" s="30"/>
+      <c r="F39" s="30"/>
+      <c r="G39" s="30"/>
+      <c r="H39" s="30"/>
+      <c r="I39" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="J39" s="60"/>
+      <c r="J39" s="32"/>
       <c r="L39" s="21"/>
     </row>
     <row r="40" spans="3:16" x14ac:dyDescent="0.3">
@@ -1530,15 +1530,13 @@
     </row>
   </sheetData>
   <mergeCells count="29">
-    <mergeCell ref="C39:H39"/>
-    <mergeCell ref="I39:J39"/>
-    <mergeCell ref="C30:E30"/>
-    <mergeCell ref="F30:I30"/>
-    <mergeCell ref="F32:I32"/>
-    <mergeCell ref="C35:E35"/>
-    <mergeCell ref="F35:I35"/>
-    <mergeCell ref="C37:E37"/>
-    <mergeCell ref="F37:I37"/>
+    <mergeCell ref="C8:E8"/>
+    <mergeCell ref="F8:I8"/>
+    <mergeCell ref="C4:F4"/>
+    <mergeCell ref="G4:J4"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="C7:E7"/>
+    <mergeCell ref="F7:I7"/>
     <mergeCell ref="F27:I27"/>
     <mergeCell ref="C9:E9"/>
     <mergeCell ref="F9:I9"/>
@@ -1552,13 +1550,15 @@
     <mergeCell ref="C23:D23"/>
     <mergeCell ref="C25:E25"/>
     <mergeCell ref="F25:I25"/>
-    <mergeCell ref="C8:E8"/>
-    <mergeCell ref="F8:I8"/>
-    <mergeCell ref="C4:F4"/>
-    <mergeCell ref="G4:J4"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="C7:E7"/>
-    <mergeCell ref="F7:I7"/>
+    <mergeCell ref="C39:H39"/>
+    <mergeCell ref="I39:J39"/>
+    <mergeCell ref="C30:E30"/>
+    <mergeCell ref="F30:I30"/>
+    <mergeCell ref="F32:I32"/>
+    <mergeCell ref="C35:E35"/>
+    <mergeCell ref="F35:I35"/>
+    <mergeCell ref="C37:E37"/>
+    <mergeCell ref="F37:I37"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="F8" r:id="rId1" xr:uid="{24426368-5A6C-4187-9C63-3E3C53FC250F}"/>

</xml_diff>